<commit_message>
adjust : real size
</commit_message>
<xml_diff>
--- a/Power/Power BOM.xlsx
+++ b/Power/Power BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\source_code\digital_twin\Power\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source_code\digital_twin-Hradware\Power\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F56AB0A-9B36-4041-BCC8-9B32864F793A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261C9069-D2D4-4D24-AD85-D27B660D98B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8ACD1470-CBC6-4DF3-97B4-6B237BD97699}"/>
+    <workbookView xWindow="17400" yWindow="-75" windowWidth="21600" windowHeight="11835" xr2:uid="{1A664D5C-8E0F-4E07-BB7F-F731D9D71FC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Power BOM" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
   <si>
     <t>Description</t>
   </si>
@@ -42,6 +42,24 @@
     <t>Quantity</t>
   </si>
   <si>
+    <t>SMD Capacitor</t>
+  </si>
+  <si>
+    <t>16v 4700uf</t>
+  </si>
+  <si>
+    <t>C1, C2, C3</t>
+  </si>
+  <si>
+    <t>1206 SMD Capacitor</t>
+  </si>
+  <si>
+    <t>16v 10uf</t>
+  </si>
+  <si>
+    <t>C4, C5, C6</t>
+  </si>
+  <si>
     <t>Default Diode</t>
   </si>
   <si>
@@ -81,9 +99,6 @@
     <t>2.5 Hole Power Supply</t>
   </si>
   <si>
-    <t>PWR2.5</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
@@ -105,7 +120,7 @@
     <t>L1, L2</t>
   </si>
   <si>
-    <t>Battery Pin</t>
+    <t>Battery In Pin</t>
   </si>
   <si>
     <t>KF2EDGR-5.08 4P</t>
@@ -114,7 +129,7 @@
     <t>P1</t>
   </si>
   <si>
-    <t>Power Pin</t>
+    <t>Power Out Pin</t>
   </si>
   <si>
     <t>KF2EDGR-5.08 6P</t>
@@ -159,13 +174,10 @@
     <t>Small Power Supply</t>
   </si>
   <si>
-    <t>5V to 3P3 Power Supply</t>
-  </si>
-  <si>
     <t>T1</t>
   </si>
   <si>
-    <t>Power Supply</t>
+    <t>12V to 5V Power Supply</t>
   </si>
   <si>
     <t>PSD-30C-5</t>
@@ -174,10 +186,21 @@
     <t>T2</t>
   </si>
   <si>
+    <t>12V to 12V Power Supply</t>
+  </si>
+  <si>
     <t>XH-M401</t>
   </si>
   <si>
     <t>T3</t>
+  </si>
+  <si>
+    <t>還沒買</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>等貨到測試</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -201,7 +224,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,14 +237,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -244,18 +261,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -263,7 +294,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -579,274 +610,327 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB05EC06-011A-497B-B872-2988C392A92F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595B9812-9BEE-4FEE-8EC7-9A37220B427F}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.625" customWidth="1"/>
+    <col min="3" max="3" width="10.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="D2" s="4">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D3" s="4">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="E11" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="4">
+        <v>1</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="3">
-        <v>1</v>
+      <c r="B19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>